<commit_message>
[Nico] - Sim-Trial v1.3 - Cross-Entropy Error defined
</commit_message>
<xml_diff>
--- a/excels/classif.xlsx
+++ b/excels/classif.xlsx
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t xml:space="preserve">Primary Author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference</t>
   </si>
   <si>
     <t xml:space="preserve">Robot Type</t>
@@ -331,7 +328,10 @@
     <t xml:space="preserve">Quality of observation</t>
   </si>
   <si>
-    <t xml:space="preserve">Flat – observation objects</t>
+    <t xml:space="preserve">Flat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation objects</t>
   </si>
   <si>
     <t xml:space="preserve">submaps</t>
@@ -566,7 +566,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -601,6 +601,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -652,7 +657,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -662,6 +667,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -682,26 +691,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+      <selection pane="bottomLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -720,25 +730,25 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -747,10 +757,10 @@
       <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
@@ -765,27 +775,27 @@
       <c r="K2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>24</v>
@@ -800,74 +810,74 @@
         <v>27</v>
       </c>
       <c r="I5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="F7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="0" t="s">
+      <c r="J8" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="0" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="0" t="s">
+      <c r="J9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="0" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="0" t="s">
+      <c r="J10" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="B11" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>41</v>
+      <c r="C11" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>42</v>
@@ -887,79 +897,79 @@
       <c r="K11" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="0" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="C14" s="0" t="s">
         <v>51</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="F14" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="J14" s="0" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>57</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="F16" s="0" t="s">
         <v>59</v>
       </c>
       <c r="G16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="C18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>64</v>
@@ -973,31 +983,31 @@
       <c r="I18" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="K18" s="0" t="n">
+      <c r="J18" s="0" t="n">
         <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>71</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>73</v>
@@ -1008,28 +1018,28 @@
       <c r="J20" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="K20" s="0" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>79</v>
       </c>
       <c r="F22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="0" t="s">
         <v>80</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>81</v>
@@ -1037,54 +1047,54 @@
       <c r="I22" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="J22" s="0" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="C24" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="E24" s="0" t="s">
         <v>86</v>
       </c>
       <c r="F24" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>88</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="C26" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>92</v>
@@ -1092,12 +1102,12 @@
       <c r="I26" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="J26" s="0" t="s">
+      <c r="J26" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="0" t="s">
+      <c r="E27" s="0" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1108,30 +1118,30 @@
       <c r="B28" s="0" t="s">
         <v>97</v>
       </c>
+      <c r="C28" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="D28" s="0" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I29" s="0" t="s">
+      <c r="H29" s="0" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1142,26 +1152,26 @@
       <c r="B30" s="0" t="s">
         <v>102</v>
       </c>
+      <c r="C30" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="D30" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="F30" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,23 +1181,23 @@
       <c r="B32" s="0" t="s">
         <v>106</v>
       </c>
+      <c r="C32" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="D32" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="F32" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="G32" s="0" t="s">
+        <v>108</v>
+      </c>
       <c r="H32" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1197,26 +1207,26 @@
       <c r="B34" s="0" t="s">
         <v>111</v>
       </c>
+      <c r="C34" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="D34" s="0" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,31 +1236,31 @@
       <c r="B36" s="0" t="s">
         <v>115</v>
       </c>
+      <c r="C36" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="D36" s="0" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="L36" s="0" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1261,28 +1271,28 @@
       <c r="B38" s="0" t="s">
         <v>120</v>
       </c>
+      <c r="C38" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="D38" s="0" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>121</v>
+        <v>42</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="K38" s="0" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1293,28 +1303,28 @@
       <c r="B40" s="0" t="s">
         <v>127</v>
       </c>
+      <c r="C40" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="D40" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="F40" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="K40" s="0" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1325,54 +1335,54 @@
       <c r="B42" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="C42" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="D42" s="0" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>131</v>
+        <v>25</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>133</v>
+        <v>24</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L42" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="M42" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="N42" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="O42" s="0" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="0" t="s">
+        <v>139</v>
+      </c>
       <c r="F43" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="G43" s="0" t="s">
         <v>140</v>
       </c>
+      <c r="L43" s="0" t="s">
+        <v>141</v>
+      </c>
       <c r="M43" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="N43" s="0" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1383,31 +1393,31 @@
       <c r="B44" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="C44" s="0" t="s">
+        <v>51</v>
+      </c>
       <c r="D44" s="0" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>131</v>
+        <v>25</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="L44" s="0" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1418,28 +1428,28 @@
       <c r="B46" s="0" t="s">
         <v>149</v>
       </c>
+      <c r="C46" s="0" t="s">
+        <v>10</v>
+      </c>
       <c r="D46" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="I46" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G46" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>151</v>
-      </c>
       <c r="J46" s="0" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="L46" s="0" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1450,7 +1460,7 @@
       <c r="B47" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="K47" s="0" t="s">
+      <c r="J47" s="0" t="s">
         <v>155</v>
       </c>
     </row>
@@ -1461,31 +1471,31 @@
       <c r="B49" s="0" t="s">
         <v>157</v>
       </c>
+      <c r="C49" s="0" t="s">
+        <v>57</v>
+      </c>
       <c r="D49" s="0" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>12</v>
+        <v>158</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>158</v>
+        <v>42</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>43</v>
+        <v>159</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>160</v>
+        <v>82</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>83</v>
+        <v>161</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="L49" s="0" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1496,28 +1506,28 @@
       <c r="B51" s="0" t="s">
         <v>164</v>
       </c>
+      <c r="C51" s="0" t="s">
+        <v>165</v>
+      </c>
       <c r="D51" s="0" t="s">
-        <v>165</v>
+        <v>11</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>107</v>
+        <v>166</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>168</v>
+        <v>82</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="K51" s="0" t="s">
         <v>169</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Nico] - Writing v0.2 - First Drafts
</commit_message>
<xml_diff>
--- a/excels/classif.xlsx
+++ b/excels/classif.xlsx
@@ -493,7 +493,7 @@
     <t xml:space="preserve">also called object/area</t>
   </si>
   <si>
-    <t xml:space="preserve"> KNOWROB-MAP - knowledge-linked semantic object maps </t>
+    <t xml:space="preserve">KNOWROB-MAP - knowledge-linked semantic object maps </t>
   </si>
   <si>
     <t xml:space="preserve">D. Tenorth</t>
@@ -566,7 +566,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -601,11 +601,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -657,7 +652,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -667,10 +662,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -693,10 +684,10 @@
   </sheetPr>
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1102,7 +1093,7 @@
       <c r="I26" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J26" s="2" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Nico] - Writing v0.3 - Lit Refined
</commit_message>
<xml_diff>
--- a/excels/classif.xlsx
+++ b/excels/classif.xlsx
@@ -680,19 +680,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="62.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
@@ -1525,7 +1525,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="2" fitToHeight="2" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[Nico] - Writing v0.5 - Added results image
</commit_message>
<xml_diff>
--- a/excels/classif.xlsx
+++ b/excels/classif.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="207">
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -790,31 +793,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:O83"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F75" activeCellId="0" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="62.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -832,29 +836,32 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>9</v>
+      <c r="A2" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>2010</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>12</v>
@@ -862,10 +869,10 @@
       <c r="F2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="0" t="s">
@@ -880,33 +887,37 @@
       <c r="L2" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="M2" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="L3" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>23</v>
+      <c r="A5" s="0" t="n">
+        <f aca="false">A2+1</f>
+        <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>2008</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>26</v>
@@ -921,85 +932,93 @@
         <v>29</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>20</v>
+      <c r="C6" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>31</v>
+      <c r="A8" s="0" t="n">
+        <f aca="false">A5+1</f>
+        <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="E8" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="H8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="L9" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="0" t="s">
+      <c r="G10" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="L10" s="0" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" s="0" t="s">
+      <c r="G11" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="L11" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>41</v>
+      <c r="A13" s="0" t="n">
+        <f aca="false">A8+1</f>
+        <v>4</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="0" t="n">
         <v>2020</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>44</v>
@@ -1019,42 +1038,46 @@
       <c r="L13" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="M13" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>50</v>
+      <c r="C14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>51</v>
+      <c r="A16" s="0" t="n">
+        <f aca="false">A13+1</f>
+        <v>5</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="0" t="n">
         <v>2018</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E16" s="0" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="J16" s="0" t="s">
         <v>56</v>
@@ -1062,35 +1085,39 @@
       <c r="K16" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="L16" s="0" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
-        <v>58</v>
+      <c r="C17" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>59</v>
+      <c r="C18" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>60</v>
+      <c r="A20" s="0" t="n">
+        <f aca="false">A16+1</f>
+        <v>6</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="0" t="n">
         <v>1995</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="E20" s="0" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>64</v>
@@ -1107,78 +1134,86 @@
       <c r="K20" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="L20" s="0" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>27</v>
+      <c r="C21" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>71</v>
       </c>
+      <c r="J21" s="0" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>44</v>
+      <c r="C22" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>73</v>
+      <c r="A24" s="0" t="n">
+        <f aca="false">A20+1</f>
+        <v>7</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="0" t="n">
         <v>2015</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="E24" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>76</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>77</v>
+        <v>16</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>20</v>
+      <c r="C25" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>78</v>
+      <c r="A27" s="0" t="n">
+        <f aca="false">A24+1</f>
+        <v>8</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="0" t="n">
         <v>2018</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="E27" s="0" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>81</v>
@@ -1192,39 +1227,43 @@
       <c r="J27" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="K27" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="L27" s="0" t="n">
         <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
-        <v>20</v>
+      <c r="C28" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>85</v>
+      <c r="A30" s="0" t="n">
+        <f aca="false">A27+1</f>
+        <v>9</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="0" t="n">
         <v>2017</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E30" s="0" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>88</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>90</v>
@@ -1235,36 +1274,40 @@
       <c r="K30" s="0" t="s">
         <v>92</v>
       </c>
+      <c r="L30" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
-        <v>20</v>
+      <c r="C31" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>93</v>
+      <c r="A33" s="0" t="n">
+        <f aca="false">A30+1</f>
+        <v>10</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C33" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="0" t="n">
         <v>2013</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E33" s="0" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>96</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="I33" s="0" t="s">
         <v>98</v>
@@ -1272,73 +1315,81 @@
       <c r="J33" s="0" t="s">
         <v>99</v>
       </c>
+      <c r="K33" s="0" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>100</v>
+      <c r="C34" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>101</v>
+      <c r="A36" s="0" t="n">
+        <f aca="false">A33+1</f>
+        <v>11</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="0" t="n">
         <v>2019</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="F36" s="0" t="s">
+      <c r="E36" s="0" t="s">
         <v>104</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>106</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>57</v>
+        <v>100</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
-        <v>20</v>
+      <c r="C37" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>107</v>
+      <c r="A39" s="0" t="n">
+        <f aca="false">A36+1</f>
+        <v>12</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="0" t="n">
         <v>2015</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E39" s="0" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="I39" s="0" t="s">
         <v>110</v>
@@ -1346,273 +1397,297 @@
       <c r="J39" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="K39" s="0" t="s">
         <v>112</v>
       </c>
+      <c r="L39" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="F40" s="0" t="s">
+      <c r="C40" s="0" t="s">
         <v>114</v>
       </c>
+      <c r="G40" s="0" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
-        <v>115</v>
+      <c r="C41" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>116</v>
+      <c r="A43" s="0" t="n">
+        <f aca="false">A39+1</f>
+        <v>13</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C43" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="0" t="n">
         <v>2016</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E43" s="0" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="I44" s="0" t="s">
+      <c r="C44" s="0" t="s">
         <v>122</v>
       </c>
+      <c r="J44" s="0" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
-        <v>123</v>
+      <c r="C45" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>124</v>
+      <c r="A47" s="0" t="n">
+        <f aca="false">A43+1</f>
+        <v>14</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C47" s="0" t="n">
+      <c r="C47" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" s="0" t="n">
         <v>2017</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E47" s="0" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>126</v>
+        <v>55</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>127</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>128</v>
+        <v>100</v>
+      </c>
+      <c r="L47" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="s">
-        <v>129</v>
+      <c r="C48" s="0" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>130</v>
+      <c r="A50" s="0" t="n">
+        <f aca="false">A47+1</f>
+        <v>15</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C50" s="0" t="n">
+      <c r="C50" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="0" t="n">
         <v>2017</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E50" s="0" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="H50" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G50" s="0" t="s">
         <v>133</v>
       </c>
       <c r="I50" s="0" t="s">
         <v>134</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>135</v>
+        <v>100</v>
+      </c>
+      <c r="L50" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
-        <v>136</v>
+      <c r="C51" s="0" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
-        <v>137</v>
+      <c r="C52" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>138</v>
+      <c r="A54" s="0" t="n">
+        <f aca="false">A50+1</f>
+        <v>16</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="C54" s="0" t="n">
+      <c r="C54" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D54" s="0" t="n">
         <v>2017</v>
       </c>
-      <c r="D54" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E54" s="0" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="I54" s="0" t="s">
         <v>141</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="K54" s="0" t="s">
-        <v>57</v>
+        <v>100</v>
+      </c>
+      <c r="L54" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
-        <v>142</v>
+      <c r="C55" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
-        <v>143</v>
+      <c r="C56" s="0" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>144</v>
+      <c r="A58" s="0" t="n">
+        <f aca="false">A54+1</f>
+        <v>17</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="C58" s="0" t="n">
+      <c r="C58" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D58" s="0" t="n">
         <v>2018</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E58" s="0" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>146</v>
+        <v>16</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="K58" s="0" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="L58" s="0" t="s">
         <v>148</v>
       </c>
+      <c r="M58" s="0" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="K59" s="0" t="s">
-        <v>57</v>
+      <c r="C59" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="L59" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
-        <v>150</v>
+      <c r="C60" s="0" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>151</v>
+      <c r="A62" s="0" t="n">
+        <f aca="false">A58+1</f>
+        <v>18</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="C62" s="0" t="n">
+      <c r="C62" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D62" s="0" t="n">
         <v>2019</v>
       </c>
-      <c r="D62" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E62" s="0" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>153</v>
+        <v>96</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>154</v>
+        <v>45</v>
       </c>
       <c r="I62" s="0" t="s">
         <v>155</v>
@@ -1623,93 +1698,101 @@
       <c r="K62" s="0" t="s">
         <v>157</v>
       </c>
+      <c r="L62" s="0" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="K63" s="0" t="s">
-        <v>120</v>
+      <c r="C63" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="L63" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="0" t="s">
-        <v>159</v>
+      <c r="C64" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>160</v>
+      <c r="A66" s="0" t="n">
+        <f aca="false">A62+1</f>
+        <v>19</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="C66" s="0" t="n">
+      <c r="C66" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D66" s="0" t="n">
         <v>2018</v>
       </c>
-      <c r="D66" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E66" s="0" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="K66" s="0" t="s">
-        <v>162</v>
+        <v>100</v>
+      </c>
+      <c r="L66" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0" t="s">
+      <c r="C67" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <f aca="false">A66+1</f>
         <v>20</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="C69" s="0" t="n">
+      <c r="C69" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D69" s="0" t="n">
         <v>2016</v>
       </c>
-      <c r="D69" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E69" s="0" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>165</v>
+        <v>96</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>166</v>
+        <v>28</v>
       </c>
       <c r="I69" s="0" t="s">
         <v>167</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>26</v>
+        <v>168</v>
       </c>
       <c r="K69" s="0" t="s">
-        <v>168</v>
+        <v>27</v>
       </c>
       <c r="L69" s="0" t="s">
         <v>169</v>
@@ -1723,54 +1806,58 @@
       <c r="O69" s="0" t="s">
         <v>172</v>
       </c>
+      <c r="P69" s="0" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>173</v>
+      <c r="C70" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="K70" s="0" t="s">
+      <c r="H70" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="M70" s="0" t="s">
+      <c r="L70" s="0" t="s">
         <v>176</v>
       </c>
       <c r="N70" s="0" t="s">
         <v>177</v>
       </c>
+      <c r="O70" s="0" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>178</v>
+      <c r="A72" s="0" t="n">
+        <f aca="false">A69+1</f>
+        <v>21</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="C72" s="0" t="n">
+        <v>179</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D72" s="0" t="n">
         <v>2018</v>
       </c>
-      <c r="D72" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="E72" s="0" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>165</v>
+        <v>96</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>166</v>
+        <v>28</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="J72" s="0" t="s">
         <v>180</v>
@@ -1781,130 +1868,146 @@
       <c r="L72" s="0" t="s">
         <v>182</v>
       </c>
+      <c r="M72" s="0" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="s">
-        <v>20</v>
+      <c r="C73" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>183</v>
+      <c r="A75" s="0" t="n">
+        <f aca="false">A72+1</f>
+        <v>22</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="C75" s="0" t="n">
+      <c r="C75" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D75" s="0" t="n">
         <v>2011</v>
       </c>
-      <c r="D75" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="E75" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G75" s="0" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>185</v>
+        <v>28</v>
       </c>
       <c r="I75" s="0" t="s">
         <v>186</v>
       </c>
       <c r="J75" s="0" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="K75" s="0" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="L75" s="0" t="s">
-        <v>187</v>
+        <v>48</v>
+      </c>
+      <c r="M75" s="0" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="s">
-        <v>20</v>
+      <c r="C76" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>188</v>
+      <c r="A77" s="0" t="n">
+        <f aca="false">A75+1</f>
+        <v>23</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C77" s="0" t="n">
+      <c r="C77" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="D77" s="0" t="n">
         <v>2018</v>
       </c>
-      <c r="K77" s="0" t="s">
-        <v>190</v>
+      <c r="L77" s="0" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>191</v>
+      <c r="A79" s="0" t="n">
+        <f aca="false">A77+1</f>
+        <v>24</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="C79" s="0" t="n">
+      <c r="C79" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="D79" s="0" t="n">
         <v>2018</v>
       </c>
-      <c r="D79" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="E79" s="0" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>193</v>
+        <v>13</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>44</v>
+        <v>194</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="I79" s="0" t="s">
         <v>195</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="K79" s="0" t="s">
-        <v>196</v>
+        <v>100</v>
       </c>
       <c r="L79" s="0" t="s">
         <v>197</v>
       </c>
+      <c r="M79" s="0" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0" t="s">
-        <v>20</v>
+      <c r="C80" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>198</v>
+      <c r="A82" s="0" t="n">
+        <f aca="false">A79+1</f>
+        <v>25</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="C82" s="0" t="n">
+      <c r="C82" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="D82" s="0" t="n">
         <v>2010</v>
       </c>
-      <c r="D82" s="0" t="s">
-        <v>200</v>
-      </c>
       <c r="E82" s="0" t="s">
-        <v>12</v>
+        <v>201</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>132</v>
+        <v>13</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>201</v>
+        <v>133</v>
       </c>
       <c r="H82" s="0" t="s">
         <v>202</v>
@@ -1913,15 +2016,18 @@
         <v>203</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>99</v>
+        <v>204</v>
       </c>
       <c r="K82" s="0" t="s">
-        <v>204</v>
+        <v>100</v>
+      </c>
+      <c r="L82" s="0" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="0" t="s">
-        <v>205</v>
+      <c r="C83" s="0" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Nico] - Writing v.0.6 - Latex Error
</commit_message>
<xml_diff>
--- a/excels/classif.xlsx
+++ b/excels/classif.xlsx
@@ -796,9 +796,9 @@
   <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F75" activeCellId="0" sqref="F75"/>
+      <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>